<commit_message>
updated with Fernandina duplicate
</commit_message>
<xml_diff>
--- a/Holocene_Volcanoes_volcdef_cfg.xlsx
+++ b/Holocene_Volcanoes_volcdef_cfg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/famelung/code/minsar/tools/VolcDef_web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092264B0-AAF5-7140-A799-88506B5670C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5AC24D-61E9-9647-B03C-2E6A41D3D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="660" windowWidth="29500" windowHeight="19160" xr2:uid="{C0385577-DB88-5B46-BC32-5548AF298521}"/>
   </bookViews>
@@ -6448,7 +6448,7 @@
   <dimension ref="A1:N1327"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1059" workbookViewId="0">
-      <selection activeCell="A1079" sqref="A1079"/>
+      <selection activeCell="B1079" sqref="B1079"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53830,7 +53830,7 @@
     </row>
     <row r="1078" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1078" s="5" t="s">
-        <v>1980</v>
+        <v>1983</v>
       </c>
       <c r="B1078" s="3">
         <v>353010</v>
@@ -53874,7 +53874,7 @@
     </row>
     <row r="1079" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1079" s="5" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="B1079" s="3">
         <v>353010</v>

</xml_diff>